<commit_message>
Excel styling is done
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="2020-05-10" sheetId="1" r:id="rId4"/>
@@ -268,7 +268,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,15 +278,74 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="dddddd"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border/>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -588,10 +647,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A38" sqref="A38:L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -600,7 +659,7 @@
       <c r="J1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -608,9 +667,10 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:13">
       <c r="J3" t="s">
@@ -621,201 +681,344 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
         <v>100</v>
       </c>
-      <c r="H4" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>10000</v>
       </c>
-      <c r="H5" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K5" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>5000</v>
       </c>
-      <c r="D6"/>
-      <c r="H6" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K6" t="s">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="B7">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
         <v>8000</v>
       </c>
-      <c r="D7"/>
-      <c r="H7" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K7" t="s">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>3000</v>
       </c>
-      <c r="D8"/>
-      <c r="H8" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K8" t="s">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D9"/>
-      <c r="J9" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="J9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K9"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D10"/>
-      <c r="J10" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K10"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11"/>
-      <c r="J11" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K11"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D12"/>
-      <c r="J12" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="J12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K12"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D13">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2">
         <v>100</v>
       </c>
-      <c r="J13" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K13"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <v>0</v>
       </c>
-      <c r="J14" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="J14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K14"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>31</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J16"/>
-      <c r="M16" t="s">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="B17" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F17" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J17" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6" t="s">
         <v>36</v>
       </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B18" s="2">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E18" t="s">
+      <c r="D18" s="2">
+        <v>200</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G18" t="s">
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I18" t="s">
+      <c r="H18" s="2">
+        <v>300</v>
+      </c>
+      <c r="I18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K18" t="s">
+      <c r="J18" s="2">
+        <v>3</v>
+      </c>
+      <c r="K18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M18" t="s">
+      <c r="L18" s="2">
+        <v>3000</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K19" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="2">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M19" t="s">
+      <c r="L19" s="2">
+        <v>2000</v>
+      </c>
+      <c r="M19" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K20" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="2">
+        <v>5</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M20" t="s">
+      <c r="L20" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -933,11 +1136,79 @@
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
+    <mergeCell ref="C2:C2"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="H4:M4"/>
@@ -992,6 +1263,8 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="K26:L26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="K27:L27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="E28:F28"/>
@@ -1035,10 +1308,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A39" sqref="A39:L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1047,7 +1320,7 @@
       <c r="J1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1055,9 +1328,10 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:13">
       <c r="J3" t="s">
@@ -1068,213 +1342,365 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K5" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="D6"/>
-      <c r="H6" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K6" t="s">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13">
-      <c r="B7">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
         <v>1</v>
       </c>
-      <c r="D7"/>
-      <c r="H7" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K7" t="s">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>1</v>
       </c>
-      <c r="D8"/>
-      <c r="H8" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K8" t="s">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="B9">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="D9"/>
-      <c r="H9" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K9" t="s">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10"/>
-      <c r="J10" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="J10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K10"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11"/>
-      <c r="J11" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="J11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K11"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12"/>
-      <c r="J12" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="J12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K12"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13"/>
-      <c r="J13" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="J13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K13"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D14">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2">
         <v>2</v>
       </c>
-      <c r="J14" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="J14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K14"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2">
         <v>4</v>
       </c>
-      <c r="J15" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K15"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J17"/>
-      <c r="M17" t="s">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="B18" t="s">
+      <c r="A18" s="2"/>
+      <c r="B18" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F18" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J18" t="s">
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6" t="s">
         <v>36</v>
       </c>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E19" t="s">
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G19" t="s">
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I19" t="s">
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K19" t="s">
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M19" t="s">
+      <c r="L19" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M19" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K20" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="2">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M20" t="s">
+      <c r="L20" s="2">
+        <v>500</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K21" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="M21" t="s">
+      <c r="L21" s="2">
+        <v>200</v>
+      </c>
+      <c r="M21" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1392,11 +1818,79 @@
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
+    <mergeCell ref="C2:C2"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="H4:M4"/>
@@ -1455,6 +1949,8 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="K27:L27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="K28:L28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E29:F29"/>

</xml_diff>

<commit_message>
edit.php is updated. Now a user can edit between 記入者 and 翌日預け入れ .
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="2020-05-10" sheetId="1" r:id="rId4"/>
-    <sheet name="2020-05-12" sheetId="2" r:id="rId5"/>
+    <sheet name="2020-06-01" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -16,18 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
   <si>
     <t>記入者</t>
   </si>
   <si>
-    <t>tadashi</t>
+    <t>tom</t>
   </si>
   <si>
     <t>日付</t>
   </si>
   <si>
-    <t>2020-05-10</t>
+    <t>2020-06-01</t>
   </si>
   <si>
     <t>店舗名</t>
@@ -54,25 +53,25 @@
     <t>入金</t>
   </si>
   <si>
-    <t>Nクラブ</t>
-  </si>
-  <si>
-    <t>シューズ</t>
-  </si>
-  <si>
-    <t>Sクラブ</t>
-  </si>
-  <si>
-    <t>ボール</t>
+    <t>wjosdin</t>
+  </si>
+  <si>
+    <t>kdンフォあいd</t>
   </si>
   <si>
     <t>出金</t>
   </si>
   <si>
-    <t>ナイキ</t>
-  </si>
-  <si>
-    <t>ボール。シューズ</t>
+    <t>hdasiobf</t>
+  </si>
+  <si>
+    <t>いアンフィえ</t>
+  </si>
+  <si>
+    <t>hf0位あんfd</t>
+  </si>
+  <si>
+    <t>おアンフィ</t>
   </si>
   <si>
     <t>支払計</t>
@@ -144,31 +143,34 @@
     <t>売掛金</t>
   </si>
   <si>
-    <t>岡部様</t>
-  </si>
-  <si>
-    <t>3000円</t>
-  </si>
-  <si>
-    <t>佐々木様</t>
-  </si>
-  <si>
-    <t>4000円</t>
+    <t>irehai様</t>
+  </si>
+  <si>
+    <t>222円</t>
+  </si>
+  <si>
+    <t>dfoianf様</t>
+  </si>
+  <si>
+    <t>3333円</t>
   </si>
   <si>
     <t>DC売上内訳</t>
   </si>
   <si>
-    <t>1000円</t>
+    <t>49549円</t>
   </si>
   <si>
     <t>JCB売上内訳</t>
   </si>
   <si>
-    <t>2000円</t>
-  </si>
-  <si>
-    <t>2500円</t>
+    <t>2020円</t>
+  </si>
+  <si>
+    <t>8484円</t>
+  </si>
+  <si>
+    <t>383838円</t>
   </si>
   <si>
     <t>DC売上合計</t>
@@ -177,79 +179,40 @@
     <t>2件</t>
   </si>
   <si>
+    <t>58033円</t>
+  </si>
+  <si>
     <t>JCB売上合計</t>
   </si>
   <si>
-    <t>5500円</t>
+    <t>385858円</t>
   </si>
   <si>
     <t>PAYPAY売上合計</t>
   </si>
   <si>
+    <t>23333円</t>
+  </si>
+  <si>
+    <t>nanaco</t>
+  </si>
+  <si>
     <t>3件</t>
   </si>
   <si>
-    <t>4500円</t>
-  </si>
-  <si>
-    <t>nanaco</t>
-  </si>
-  <si>
-    <t>300円</t>
+    <t>3円</t>
   </si>
   <si>
     <t>suica</t>
   </si>
   <si>
-    <t>6件</t>
-  </si>
-  <si>
     <t>edy</t>
   </si>
   <si>
-    <t>4件</t>
-  </si>
-  <si>
     <t>その他交通IC</t>
   </si>
   <si>
     <t>メモ、伝達事項：</t>
-  </si>
-  <si>
-    <t>goerge</t>
-  </si>
-  <si>
-    <t>2020-05-12</t>
-  </si>
-  <si>
-    <t>ふ</t>
-  </si>
-  <si>
-    <t>じ</t>
-  </si>
-  <si>
-    <t>ほほほ</t>
-  </si>
-  <si>
-    <t>チョコレート</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>deded</t>
-  </si>
-  <si>
-    <t>1円</t>
-  </si>
-  <si>
-    <t>2円</t>
-  </si>
-  <si>
-    <t>3円</t>
-  </si>
-  <si>
-    <t>1件</t>
   </si>
 </sst>
 </file>
@@ -647,667 +610,6 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:M42"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A38" sqref="A38:L42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="J3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2">
-        <v>100</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2">
-        <v>10000</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5000</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2">
-        <v>8000</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="2">
-        <v>3000</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="J9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="J10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="J11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="J12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2">
-        <v>100</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="J13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="J14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" s="2"/>
-      <c r="B17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="2">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2">
-        <v>200</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="2">
-        <v>2</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="2">
-        <v>300</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="2">
-        <v>3</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L18" s="2">
-        <v>3000</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="2">
-        <v>4</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L19" s="2">
-        <v>2000</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="2">
-        <v>5</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L20" s="2">
-        <v>1000</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" t="s">
-        <v>48</v>
-      </c>
-      <c r="K26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="E27" t="s">
-        <v>49</v>
-      </c>
-      <c r="K27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" t="s">
-        <v>43</v>
-      </c>
-      <c r="G28" t="s">
-        <v>53</v>
-      </c>
-      <c r="I28" t="s">
-        <v>52</v>
-      </c>
-      <c r="K28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E34" t="s">
-        <v>59</v>
-      </c>
-      <c r="G34" t="s">
-        <v>60</v>
-      </c>
-      <c r="I34" t="s">
-        <v>61</v>
-      </c>
-      <c r="K34" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" t="s">
-        <v>63</v>
-      </c>
-      <c r="E35" t="s">
-        <v>40</v>
-      </c>
-      <c r="G35" t="s">
-        <v>64</v>
-      </c>
-      <c r="I35"/>
-      <c r="K35"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
-    <mergeCell ref="C2:C2"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:M4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="A8:A8"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:L42"/>
-  </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
@@ -1321,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1329,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1348,7 +650,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1369,7 +671,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>40000</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1390,7 +692,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2">
-        <v>1</v>
+        <v>3944</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -1398,12 +700,12 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2" t="s">
-        <v>69</v>
+      <c r="K6" s="2">
+        <v>2884</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
@@ -1411,7 +713,7 @@
     <row r="7" spans="1:13">
       <c r="A7" s="2"/>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>3393</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1419,22 +721,22 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2" t="s">
-        <v>70</v>
+      <c r="K7" s="2">
+        <v>59494</v>
       </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
-        <v>1</v>
+        <v>39393</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1442,12 +744,12 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1455,7 +757,7 @@
     <row r="9" spans="1:13">
       <c r="A9" s="2"/>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>38383</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1463,12 +765,12 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -1546,7 +848,7 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2">
-        <v>2</v>
+        <v>4949</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1565,7 +867,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2">
-        <v>4</v>
+        <v>393</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1618,37 +920,37 @@
         <v>37</v>
       </c>
       <c r="B19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="2">
-        <v>1</v>
+        <v>3333</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="H19" s="2">
-        <v>1</v>
+        <v>3333</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="J19" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L19" s="2">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>33</v>
@@ -1667,13 +969,13 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L20" s="2">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>33</v>
@@ -1692,13 +994,13 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>38</v>
       </c>
       <c r="L21" s="2">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>33</v>
@@ -1712,7 +1014,7 @@
         <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1720,7 +1022,7 @@
         <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1728,83 +1030,83 @@
         <v>46</v>
       </c>
       <c r="E27" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="G27" t="s">
         <v>48</v>
       </c>
       <c r="K27" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="E28" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="K28" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="G29" t="s">
+        <v>55</v>
+      </c>
+      <c r="I29" t="s">
         <v>53</v>
       </c>
-      <c r="I29" t="s">
-        <v>52</v>
-      </c>
       <c r="K29" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="G35" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" t="s">
         <v>60</v>
       </c>
-      <c r="I35" t="s">
-        <v>77</v>
-      </c>
       <c r="K35" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E36" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="G36" t="s">
         <v>64</v>

</xml_diff>